<commit_message>
separate into two levels - 5 days and annual model
</commit_message>
<xml_diff>
--- a/data_uploads/rain_rate_mm_m2.xlsx
+++ b/data_uploads/rain_rate_mm_m2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yuezi/Documents/GitHub/Regional_irrigation_energy_model/data_uploads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C293C23F-9D81-7D4C-8914-889E4F7190C7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C3C8E9E-0B6B-D541-BE9A-B9E13484A361}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1160" yWindow="1100" windowWidth="27640" windowHeight="15780" xr2:uid="{001E87E6-C378-2B43-90AE-5075B2FFED12}"/>
+    <workbookView xWindow="31760" yWindow="4540" windowWidth="27640" windowHeight="15780" xr2:uid="{001E87E6-C378-2B43-90AE-5075B2FFED12}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -66,8 +66,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -384,8 +387,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54A8F3AD-A1CA-9742-9A24-D8E019E5DA5F}">
   <dimension ref="A1:B366"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E361" sqref="E361"/>
+    <sheetView tabSelected="1" topLeftCell="A349" workbookViewId="0">
+      <selection activeCell="E358" sqref="E358"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -405,647 +408,647 @@
       <c r="A2">
         <v>20140701</v>
       </c>
-      <c r="B2">
-        <v>0</v>
+      <c r="B2" s="1">
+        <v>1.4370000000000001</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>20140702</v>
       </c>
-      <c r="B3">
-        <v>0</v>
+      <c r="B3" s="1">
+        <v>2.4580000000000002</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>20140703</v>
       </c>
-      <c r="B4">
-        <v>0</v>
+      <c r="B4" s="1">
+        <v>5.7830000000000004</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>20140704</v>
       </c>
-      <c r="B5">
-        <v>0</v>
+      <c r="B5" s="1">
+        <v>8.8960000000000008</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>20140705</v>
       </c>
-      <c r="B6">
-        <v>0</v>
+      <c r="B6" s="1">
+        <v>18.664999999999999</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>20140706</v>
       </c>
-      <c r="B7">
-        <v>0</v>
+      <c r="B7" s="1">
+        <v>5.2409999999999997</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>20140707</v>
       </c>
-      <c r="B8">
-        <v>0</v>
+      <c r="B8" s="1">
+        <v>7.258</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>20140708</v>
       </c>
-      <c r="B9">
-        <v>0</v>
+      <c r="B9" s="1">
+        <v>10.287000000000001</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>20140709</v>
       </c>
-      <c r="B10">
-        <v>0</v>
+      <c r="B10" s="1">
+        <v>5.73</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>20140710</v>
       </c>
-      <c r="B11">
-        <v>0</v>
+      <c r="B11" s="1">
+        <v>5.72</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>20140711</v>
       </c>
-      <c r="B12">
-        <v>0</v>
+      <c r="B12" s="1">
+        <v>10.218999999999999</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>20140712</v>
       </c>
-      <c r="B13">
-        <v>0</v>
+      <c r="B13" s="1">
+        <v>1.323</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>20140713</v>
       </c>
-      <c r="B14">
-        <v>0</v>
+      <c r="B14" s="1">
+        <v>2.383</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>20140714</v>
       </c>
-      <c r="B15">
-        <v>0</v>
+      <c r="B15" s="1">
+        <v>4.8689999999999998</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>20140715</v>
       </c>
-      <c r="B16">
-        <v>0</v>
+      <c r="B16" s="1">
+        <v>4.2809999999999997</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>20140716</v>
       </c>
-      <c r="B17">
-        <v>0</v>
+      <c r="B17" s="1">
+        <v>8.4459999999999997</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>20140717</v>
       </c>
-      <c r="B18">
-        <v>0</v>
+      <c r="B18" s="1">
+        <v>9.0640000000000001</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>20140718</v>
       </c>
-      <c r="B19">
-        <v>0</v>
+      <c r="B19" s="1">
+        <v>7.8440000000000003</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>20140719</v>
       </c>
-      <c r="B20">
-        <v>0</v>
+      <c r="B20" s="1">
+        <v>18.157</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>20140720</v>
       </c>
-      <c r="B21">
-        <v>0</v>
+      <c r="B21" s="1">
+        <v>7.4139999999999997</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>20140721</v>
       </c>
-      <c r="B22">
-        <v>0</v>
+      <c r="B22" s="1">
+        <v>11.635999999999999</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>20140722</v>
       </c>
-      <c r="B23">
-        <v>0</v>
+      <c r="B23" s="1">
+        <v>13.683</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>20140723</v>
       </c>
-      <c r="B24">
-        <v>0</v>
+      <c r="B24" s="1">
+        <v>3.2010000000000001</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>20140724</v>
       </c>
-      <c r="B25">
-        <v>0</v>
+      <c r="B25" s="1">
+        <v>6.9720000000000004</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>20140725</v>
       </c>
-      <c r="B26">
-        <v>0</v>
+      <c r="B26" s="1">
+        <v>11.561999999999999</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>20140726</v>
       </c>
-      <c r="B27">
-        <v>0</v>
+      <c r="B27" s="1">
+        <v>6.5609999999999999</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>20140727</v>
       </c>
-      <c r="B28">
-        <v>0</v>
+      <c r="B28" s="1">
+        <v>15.327</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>20140728</v>
       </c>
-      <c r="B29">
-        <v>0</v>
+      <c r="B29" s="1">
+        <v>2.6760000000000002</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>20140729</v>
       </c>
-      <c r="B30">
-        <v>0</v>
+      <c r="B30" s="1">
+        <v>8.6519999999999992</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>20140730</v>
       </c>
-      <c r="B31">
-        <v>0</v>
+      <c r="B31" s="1">
+        <v>24.893999999999998</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>20140731</v>
       </c>
-      <c r="B32">
-        <v>0</v>
+      <c r="B32" s="1">
+        <v>30.123000000000001</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>20140801</v>
       </c>
-      <c r="B33">
-        <v>0</v>
+      <c r="B33" s="1">
+        <v>19.222000000000001</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>20140802</v>
       </c>
-      <c r="B34">
-        <v>0</v>
+      <c r="B34" s="1">
+        <v>3.6309999999999998</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>20140803</v>
       </c>
-      <c r="B35">
-        <v>0</v>
+      <c r="B35" s="1">
+        <v>32.277000000000001</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>20140804</v>
       </c>
-      <c r="B36">
-        <v>0</v>
+      <c r="B36" s="1">
+        <v>9.0340000000000007</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>20140805</v>
       </c>
-      <c r="B37">
-        <v>0</v>
+      <c r="B37" s="1">
+        <v>4.5119999999999996</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>20140806</v>
       </c>
-      <c r="B38">
-        <v>0</v>
+      <c r="B38" s="1">
+        <v>18.004999999999999</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>20140807</v>
       </c>
-      <c r="B39">
-        <v>0</v>
+      <c r="B39" s="1">
+        <v>10.156000000000001</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>20140808</v>
       </c>
-      <c r="B40">
-        <v>0</v>
+      <c r="B40" s="1">
+        <v>6.4939999999999998</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>20140809</v>
       </c>
-      <c r="B41">
-        <v>0</v>
+      <c r="B41" s="1">
+        <v>13.51</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>20140810</v>
       </c>
-      <c r="B42">
-        <v>0</v>
+      <c r="B42" s="1">
+        <v>11.583</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>20140811</v>
       </c>
-      <c r="B43">
-        <v>0</v>
+      <c r="B43" s="1">
+        <v>1.2050000000000001</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>20140812</v>
       </c>
-      <c r="B44">
-        <v>0</v>
+      <c r="B44" s="1">
+        <v>6.548</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>20140813</v>
       </c>
-      <c r="B45">
-        <v>0</v>
+      <c r="B45" s="1">
+        <v>14.007</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>20140814</v>
       </c>
-      <c r="B46">
-        <v>0</v>
+      <c r="B46" s="1">
+        <v>9.6259999999999994</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>20140815</v>
       </c>
-      <c r="B47">
-        <v>0</v>
+      <c r="B47" s="1">
+        <v>2.1259999999999999</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>20140816</v>
       </c>
-      <c r="B48">
-        <v>0</v>
+      <c r="B48" s="1">
+        <v>11.055</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>20140817</v>
       </c>
-      <c r="B49">
-        <v>0</v>
+      <c r="B49" s="1">
+        <v>20.734999999999999</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>20140818</v>
       </c>
-      <c r="B50">
-        <v>0</v>
+      <c r="B50" s="1">
+        <v>17.884</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>20140819</v>
       </c>
-      <c r="B51">
-        <v>0</v>
+      <c r="B51" s="1">
+        <v>11.419</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>20140820</v>
       </c>
-      <c r="B52">
-        <v>0</v>
+      <c r="B52" s="1">
+        <v>4.3410000000000002</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>20140821</v>
       </c>
-      <c r="B53">
-        <v>0</v>
+      <c r="B53" s="1">
+        <v>7.55</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>20140822</v>
       </c>
-      <c r="B54">
-        <v>0</v>
+      <c r="B54" s="1">
+        <v>6.8090000000000002</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>20140823</v>
       </c>
-      <c r="B55">
-        <v>0</v>
+      <c r="B55" s="1">
+        <v>12.474</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A56">
         <v>20140824</v>
       </c>
-      <c r="B56">
-        <v>0</v>
+      <c r="B56" s="1">
+        <v>11.781000000000001</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A57">
         <v>20140825</v>
       </c>
-      <c r="B57">
-        <v>0</v>
+      <c r="B57" s="1">
+        <v>6.74</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A58">
         <v>20140826</v>
       </c>
-      <c r="B58">
-        <v>0</v>
+      <c r="B58" s="1">
+        <v>22.599</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A59">
         <v>20140827</v>
       </c>
-      <c r="B59">
-        <v>0</v>
+      <c r="B59" s="1">
+        <v>3.8130000000000002</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A60">
         <v>20140828</v>
       </c>
-      <c r="B60">
-        <v>0</v>
+      <c r="B60" s="1">
+        <v>15.529</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A61">
         <v>20140829</v>
       </c>
-      <c r="B61">
-        <v>0</v>
+      <c r="B61" s="1">
+        <v>6.843</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A62">
         <v>20140830</v>
       </c>
-      <c r="B62">
-        <v>0</v>
+      <c r="B62" s="1">
+        <v>19.178999999999998</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A63">
         <v>20140831</v>
       </c>
-      <c r="B63">
-        <v>0</v>
+      <c r="B63" s="1">
+        <v>4.3470000000000004</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A64">
         <v>20140901</v>
       </c>
-      <c r="B64">
-        <v>0</v>
+      <c r="B64" s="1">
+        <v>9.7989999999999995</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A65">
         <v>20140902</v>
       </c>
-      <c r="B65">
-        <v>0</v>
+      <c r="B65" s="1">
+        <v>7.8840000000000003</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A66">
         <v>20140903</v>
       </c>
-      <c r="B66">
-        <v>0</v>
+      <c r="B66" s="1">
+        <v>26.105</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A67">
         <v>20140904</v>
       </c>
-      <c r="B67">
-        <v>0</v>
+      <c r="B67" s="1">
+        <v>3.6259999999999999</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A68">
         <v>20140905</v>
       </c>
-      <c r="B68">
-        <v>0</v>
+      <c r="B68" s="1">
+        <v>4.8440000000000003</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A69">
         <v>20140906</v>
       </c>
-      <c r="B69">
-        <v>0</v>
+      <c r="B69" s="1">
+        <v>26.004999999999999</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A70">
         <v>20140907</v>
       </c>
-      <c r="B70">
-        <v>0</v>
+      <c r="B70" s="1">
+        <v>25.885000000000002</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A71">
         <v>20140908</v>
       </c>
-      <c r="B71">
-        <v>0</v>
+      <c r="B71" s="1">
+        <v>15.754</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A72">
         <v>20140909</v>
       </c>
-      <c r="B72">
-        <v>0</v>
+      <c r="B72" s="1">
+        <v>10.73</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A73">
         <v>20140910</v>
       </c>
-      <c r="B73">
-        <v>0</v>
+      <c r="B73" s="1">
+        <v>0.45200000000000001</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A74">
         <v>20140911</v>
       </c>
-      <c r="B74">
-        <v>0</v>
+      <c r="B74" s="1">
+        <v>11.654</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A75">
         <v>20140912</v>
       </c>
-      <c r="B75">
-        <v>0</v>
+      <c r="B75" s="1">
+        <v>3.6070000000000002</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A76">
         <v>20140913</v>
       </c>
-      <c r="B76">
-        <v>0</v>
+      <c r="B76" s="1">
+        <v>24.536999999999999</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A77">
         <v>20140914</v>
       </c>
-      <c r="B77">
-        <v>0</v>
+      <c r="B77" s="1">
+        <v>0.98899999999999999</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A78">
         <v>20140915</v>
       </c>
-      <c r="B78">
-        <v>0</v>
+      <c r="B78" s="1">
+        <v>9.8689999999999998</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A79">
         <v>20140916</v>
       </c>
-      <c r="B79">
-        <v>0</v>
+      <c r="B79" s="1">
+        <v>2.6259999999999999</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A80">
         <v>20140917</v>
       </c>
-      <c r="B80">
-        <v>0</v>
+      <c r="B80" s="1">
+        <v>3.9129999999999998</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A81">
         <v>20140918</v>
       </c>
-      <c r="B81">
-        <v>0</v>
+      <c r="B81" s="1">
+        <v>0.41099999999999998</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A82">
         <v>20140919</v>
       </c>
-      <c r="B82">
+      <c r="B82" s="1">
         <v>0</v>
       </c>
     </row>
@@ -1053,15 +1056,15 @@
       <c r="A83">
         <v>20140920</v>
       </c>
-      <c r="B83">
-        <v>0</v>
+      <c r="B83" s="1">
+        <v>0.22800000000000001</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A84">
         <v>20140921</v>
       </c>
-      <c r="B84">
+      <c r="B84" s="1">
         <v>0</v>
       </c>
     </row>
@@ -1069,63 +1072,63 @@
       <c r="A85">
         <v>20140922</v>
       </c>
-      <c r="B85">
-        <v>0</v>
+      <c r="B85" s="1">
+        <v>9.76</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A86">
         <v>20140923</v>
       </c>
-      <c r="B86">
-        <v>0</v>
+      <c r="B86" s="1">
+        <v>2.1999999999999999E-2</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A87">
         <v>20140924</v>
       </c>
-      <c r="B87">
-        <v>0</v>
+      <c r="B87" s="1">
+        <v>8.0690000000000008</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A88">
         <v>20140925</v>
       </c>
-      <c r="B88">
-        <v>0</v>
+      <c r="B88" s="1">
+        <v>0.14599999999999999</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A89">
         <v>20140926</v>
       </c>
-      <c r="B89">
-        <v>0</v>
+      <c r="B89" s="1">
+        <v>5.6029999999999998</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A90">
         <v>20140927</v>
       </c>
-      <c r="B90">
-        <v>0</v>
+      <c r="B90" s="1">
+        <v>4.5759999999999996</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A91">
         <v>20140928</v>
       </c>
-      <c r="B91">
-        <v>0</v>
+      <c r="B91" s="1">
+        <v>0.92300000000000004</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A92">
         <v>20140929</v>
       </c>
-      <c r="B92">
+      <c r="B92" s="1">
         <v>0</v>
       </c>
     </row>
@@ -1133,111 +1136,111 @@
       <c r="A93">
         <v>20140930</v>
       </c>
-      <c r="B93">
-        <v>0</v>
+      <c r="B93" s="1">
+        <v>3.0000000000000001E-3</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A94">
         <v>20141001</v>
       </c>
-      <c r="B94">
-        <v>0</v>
+      <c r="B94" s="1">
+        <v>0.24099999999999999</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A95">
         <v>20141002</v>
       </c>
-      <c r="B95">
-        <v>0</v>
+      <c r="B95" s="1">
+        <v>13.476000000000001</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A96">
         <v>20141003</v>
       </c>
-      <c r="B96">
-        <v>0</v>
+      <c r="B96" s="1">
+        <v>10.672000000000001</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A97">
         <v>20141004</v>
       </c>
-      <c r="B97">
-        <v>0</v>
+      <c r="B97" s="1">
+        <v>5.0789999999999997</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A98">
         <v>20141005</v>
       </c>
-      <c r="B98">
-        <v>0</v>
+      <c r="B98" s="1">
+        <v>5.899</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A99">
         <v>20141006</v>
       </c>
-      <c r="B99">
-        <v>0</v>
+      <c r="B99" s="1">
+        <v>16.652999999999999</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A100">
         <v>20141007</v>
       </c>
-      <c r="B100">
-        <v>0</v>
+      <c r="B100" s="1">
+        <v>0.85899999999999999</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A101">
         <v>20141008</v>
       </c>
-      <c r="B101">
-        <v>0</v>
+      <c r="B101" s="1">
+        <v>13.634</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A102">
         <v>20141009</v>
       </c>
-      <c r="B102">
-        <v>0</v>
+      <c r="B102" s="1">
+        <v>7.8659999999999997</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A103">
         <v>20141010</v>
       </c>
-      <c r="B103">
-        <v>0</v>
+      <c r="B103" s="1">
+        <v>4.024</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A104">
         <v>20141011</v>
       </c>
-      <c r="B104">
-        <v>0</v>
+      <c r="B104" s="1">
+        <v>2E-3</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A105">
         <v>20141012</v>
       </c>
-      <c r="B105">
-        <v>0</v>
+      <c r="B105" s="1">
+        <v>1.6E-2</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A106">
         <v>20141013</v>
       </c>
-      <c r="B106">
+      <c r="B106" s="1">
         <v>0</v>
       </c>
     </row>
@@ -1245,23 +1248,23 @@
       <c r="A107">
         <v>20141014</v>
       </c>
-      <c r="B107">
-        <v>0</v>
+      <c r="B107" s="1">
+        <v>1.1539999999999999</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A108">
         <v>20141015</v>
       </c>
-      <c r="B108">
-        <v>0</v>
+      <c r="B108" s="1">
+        <v>0.34699999999999998</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A109">
         <v>20141016</v>
       </c>
-      <c r="B109">
+      <c r="B109" s="1">
         <v>0</v>
       </c>
     </row>
@@ -1269,7 +1272,7 @@
       <c r="A110">
         <v>20141017</v>
       </c>
-      <c r="B110">
+      <c r="B110" s="1">
         <v>0</v>
       </c>
     </row>
@@ -1277,7 +1280,7 @@
       <c r="A111">
         <v>20141018</v>
       </c>
-      <c r="B111">
+      <c r="B111" s="1">
         <v>0</v>
       </c>
     </row>
@@ -1285,7 +1288,7 @@
       <c r="A112">
         <v>20141019</v>
       </c>
-      <c r="B112">
+      <c r="B112" s="1">
         <v>0</v>
       </c>
     </row>
@@ -1293,15 +1296,15 @@
       <c r="A113">
         <v>20141020</v>
       </c>
-      <c r="B113">
-        <v>0</v>
+      <c r="B113" s="1">
+        <v>3.5999999999999997E-2</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A114">
         <v>20141021</v>
       </c>
-      <c r="B114">
+      <c r="B114" s="1">
         <v>0</v>
       </c>
     </row>
@@ -1309,23 +1312,23 @@
       <c r="A115">
         <v>20141022</v>
       </c>
-      <c r="B115">
-        <v>0</v>
+      <c r="B115" s="1">
+        <v>0.80300000000000005</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A116">
         <v>20141023</v>
       </c>
-      <c r="B116">
-        <v>0</v>
+      <c r="B116" s="1">
+        <v>4.0000000000000001E-3</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A117">
         <v>20141024</v>
       </c>
-      <c r="B117">
+      <c r="B117" s="1">
         <v>0</v>
       </c>
     </row>
@@ -1333,7 +1336,7 @@
       <c r="A118">
         <v>20141025</v>
       </c>
-      <c r="B118">
+      <c r="B118" s="1">
         <v>0</v>
       </c>
     </row>
@@ -1341,7 +1344,7 @@
       <c r="A119">
         <v>20141026</v>
       </c>
-      <c r="B119">
+      <c r="B119" s="1">
         <v>0</v>
       </c>
     </row>
@@ -1349,7 +1352,7 @@
       <c r="A120">
         <v>20141027</v>
       </c>
-      <c r="B120">
+      <c r="B120" s="1">
         <v>0</v>
       </c>
     </row>
@@ -1357,7 +1360,7 @@
       <c r="A121">
         <v>20141028</v>
       </c>
-      <c r="B121">
+      <c r="B121" s="1">
         <v>0</v>
       </c>
     </row>
@@ -1365,7 +1368,7 @@
       <c r="A122">
         <v>20141029</v>
       </c>
-      <c r="B122">
+      <c r="B122" s="1">
         <v>0</v>
       </c>
     </row>
@@ -1373,7 +1376,7 @@
       <c r="A123">
         <v>20141030</v>
       </c>
-      <c r="B123">
+      <c r="B123" s="1">
         <v>0</v>
       </c>
     </row>
@@ -1381,7 +1384,7 @@
       <c r="A124">
         <v>20141031</v>
       </c>
-      <c r="B124">
+      <c r="B124" s="1">
         <v>0</v>
       </c>
     </row>
@@ -1389,7 +1392,7 @@
       <c r="A125">
         <v>20141101</v>
       </c>
-      <c r="B125">
+      <c r="B125" s="1">
         <v>0</v>
       </c>
     </row>
@@ -1397,7 +1400,7 @@
       <c r="A126">
         <v>20141102</v>
       </c>
-      <c r="B126">
+      <c r="B126" s="1">
         <v>0</v>
       </c>
     </row>
@@ -1405,7 +1408,7 @@
       <c r="A127">
         <v>20141103</v>
       </c>
-      <c r="B127">
+      <c r="B127" s="1">
         <v>0</v>
       </c>
     </row>
@@ -1413,7 +1416,7 @@
       <c r="A128">
         <v>20141104</v>
       </c>
-      <c r="B128">
+      <c r="B128" s="1">
         <v>0</v>
       </c>
     </row>
@@ -1421,7 +1424,7 @@
       <c r="A129">
         <v>20141105</v>
       </c>
-      <c r="B129">
+      <c r="B129" s="1">
         <v>0</v>
       </c>
     </row>
@@ -1429,7 +1432,7 @@
       <c r="A130">
         <v>20141106</v>
       </c>
-      <c r="B130">
+      <c r="B130" s="1">
         <v>0</v>
       </c>
     </row>
@@ -1437,7 +1440,7 @@
       <c r="A131">
         <v>20141107</v>
       </c>
-      <c r="B131">
+      <c r="B131" s="1">
         <v>0</v>
       </c>
     </row>
@@ -1445,7 +1448,7 @@
       <c r="A132">
         <v>20141108</v>
       </c>
-      <c r="B132">
+      <c r="B132" s="1">
         <v>0</v>
       </c>
     </row>
@@ -1453,7 +1456,7 @@
       <c r="A133">
         <v>20141109</v>
       </c>
-      <c r="B133">
+      <c r="B133" s="1">
         <v>0</v>
       </c>
     </row>
@@ -1461,7 +1464,7 @@
       <c r="A134">
         <v>20141110</v>
       </c>
-      <c r="B134">
+      <c r="B134" s="1">
         <v>0</v>
       </c>
     </row>
@@ -1469,15 +1472,15 @@
       <c r="A135">
         <v>20141111</v>
       </c>
-      <c r="B135">
-        <v>0</v>
+      <c r="B135" s="1">
+        <v>1.403</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A136">
         <v>20141112</v>
       </c>
-      <c r="B136">
+      <c r="B136" s="1">
         <v>0</v>
       </c>
     </row>
@@ -1485,63 +1488,63 @@
       <c r="A137">
         <v>20141113</v>
       </c>
-      <c r="B137">
-        <v>0</v>
+      <c r="B137" s="1">
+        <v>1E-3</v>
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A138">
         <v>20141114</v>
       </c>
-      <c r="B138">
-        <v>0</v>
+      <c r="B138" s="1">
+        <v>5.7000000000000002E-2</v>
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A139">
         <v>20141115</v>
       </c>
-      <c r="B139">
-        <v>0</v>
+      <c r="B139" s="1">
+        <v>3.1E-2</v>
       </c>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A140">
         <v>20141116</v>
       </c>
-      <c r="B140">
-        <v>0</v>
+      <c r="B140" s="1">
+        <v>0.39200000000000002</v>
       </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A141">
         <v>20141117</v>
       </c>
-      <c r="B141">
-        <v>0</v>
+      <c r="B141" s="1">
+        <v>10.333</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A142">
         <v>20141118</v>
       </c>
-      <c r="B142">
-        <v>0</v>
+      <c r="B142" s="1">
+        <v>0.28000000000000003</v>
       </c>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A143">
         <v>20141119</v>
       </c>
-      <c r="B143">
-        <v>0</v>
+      <c r="B143" s="1">
+        <v>1E-3</v>
       </c>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A144">
         <v>20141120</v>
       </c>
-      <c r="B144">
+      <c r="B144" s="1">
         <v>0</v>
       </c>
     </row>
@@ -1549,15 +1552,15 @@
       <c r="A145">
         <v>20141121</v>
       </c>
-      <c r="B145">
-        <v>0</v>
+      <c r="B145" s="1">
+        <v>1E-3</v>
       </c>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A146">
         <v>20141122</v>
       </c>
-      <c r="B146">
+      <c r="B146" s="1">
         <v>0</v>
       </c>
     </row>
@@ -1565,7 +1568,7 @@
       <c r="A147">
         <v>20141123</v>
       </c>
-      <c r="B147">
+      <c r="B147" s="1">
         <v>0</v>
       </c>
     </row>
@@ -1573,7 +1576,7 @@
       <c r="A148">
         <v>20141124</v>
       </c>
-      <c r="B148">
+      <c r="B148" s="1">
         <v>0</v>
       </c>
     </row>
@@ -1581,15 +1584,15 @@
       <c r="A149">
         <v>20141125</v>
       </c>
-      <c r="B149">
-        <v>0</v>
+      <c r="B149" s="1">
+        <v>1E-3</v>
       </c>
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A150">
         <v>20141126</v>
       </c>
-      <c r="B150">
+      <c r="B150" s="1">
         <v>0</v>
       </c>
     </row>
@@ -1597,7 +1600,7 @@
       <c r="A151">
         <v>20141127</v>
       </c>
-      <c r="B151">
+      <c r="B151" s="1">
         <v>0</v>
       </c>
     </row>
@@ -1605,7 +1608,7 @@
       <c r="A152">
         <v>20141128</v>
       </c>
-      <c r="B152">
+      <c r="B152" s="1">
         <v>0</v>
       </c>
     </row>
@@ -1613,7 +1616,7 @@
       <c r="A153">
         <v>20141129</v>
       </c>
-      <c r="B153">
+      <c r="B153" s="1">
         <v>0</v>
       </c>
     </row>
@@ -1621,7 +1624,7 @@
       <c r="A154">
         <v>20141130</v>
       </c>
-      <c r="B154">
+      <c r="B154" s="1">
         <v>0</v>
       </c>
     </row>
@@ -1629,7 +1632,7 @@
       <c r="A155">
         <v>20141201</v>
       </c>
-      <c r="B155">
+      <c r="B155" s="1">
         <v>0</v>
       </c>
     </row>
@@ -1637,7 +1640,7 @@
       <c r="A156">
         <v>20141202</v>
       </c>
-      <c r="B156">
+      <c r="B156" s="1">
         <v>0</v>
       </c>
     </row>
@@ -1645,7 +1648,7 @@
       <c r="A157">
         <v>20141203</v>
       </c>
-      <c r="B157">
+      <c r="B157" s="1">
         <v>0</v>
       </c>
     </row>
@@ -1653,7 +1656,7 @@
       <c r="A158">
         <v>20141204</v>
       </c>
-      <c r="B158">
+      <c r="B158" s="1">
         <v>0</v>
       </c>
     </row>
@@ -1661,7 +1664,7 @@
       <c r="A159">
         <v>20141205</v>
       </c>
-      <c r="B159">
+      <c r="B159" s="1">
         <v>0</v>
       </c>
     </row>
@@ -1669,7 +1672,7 @@
       <c r="A160">
         <v>20141206</v>
       </c>
-      <c r="B160">
+      <c r="B160" s="1">
         <v>0</v>
       </c>
     </row>
@@ -1677,7 +1680,7 @@
       <c r="A161">
         <v>20141207</v>
       </c>
-      <c r="B161">
+      <c r="B161" s="1">
         <v>0</v>
       </c>
     </row>
@@ -1685,15 +1688,15 @@
       <c r="A162">
         <v>20141208</v>
       </c>
-      <c r="B162">
-        <v>0</v>
+      <c r="B162" s="1">
+        <v>1.1359999999999999</v>
       </c>
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A163">
         <v>20141209</v>
       </c>
-      <c r="B163">
+      <c r="B163" s="1">
         <v>0</v>
       </c>
     </row>
@@ -1701,7 +1704,7 @@
       <c r="A164">
         <v>20141210</v>
       </c>
-      <c r="B164">
+      <c r="B164" s="1">
         <v>0</v>
       </c>
     </row>
@@ -1709,7 +1712,7 @@
       <c r="A165">
         <v>20141211</v>
       </c>
-      <c r="B165">
+      <c r="B165" s="1">
         <v>0</v>
       </c>
     </row>
@@ -1717,7 +1720,7 @@
       <c r="A166">
         <v>20141212</v>
       </c>
-      <c r="B166">
+      <c r="B166" s="1">
         <v>0</v>
       </c>
     </row>
@@ -1725,7 +1728,7 @@
       <c r="A167">
         <v>20141213</v>
       </c>
-      <c r="B167">
+      <c r="B167" s="1">
         <v>0</v>
       </c>
     </row>
@@ -1733,7 +1736,7 @@
       <c r="A168">
         <v>20141214</v>
       </c>
-      <c r="B168">
+      <c r="B168" s="1">
         <v>0</v>
       </c>
     </row>
@@ -1741,7 +1744,7 @@
       <c r="A169">
         <v>20141215</v>
       </c>
-      <c r="B169">
+      <c r="B169" s="1">
         <v>0</v>
       </c>
     </row>
@@ -1749,7 +1752,7 @@
       <c r="A170">
         <v>20141216</v>
       </c>
-      <c r="B170">
+      <c r="B170" s="1">
         <v>0</v>
       </c>
     </row>
@@ -1757,7 +1760,7 @@
       <c r="A171">
         <v>20141217</v>
       </c>
-      <c r="B171">
+      <c r="B171" s="1">
         <v>0</v>
       </c>
     </row>
@@ -1765,7 +1768,7 @@
       <c r="A172">
         <v>20141218</v>
       </c>
-      <c r="B172">
+      <c r="B172" s="1">
         <v>0</v>
       </c>
     </row>
@@ -1773,7 +1776,7 @@
       <c r="A173">
         <v>20141219</v>
       </c>
-      <c r="B173">
+      <c r="B173" s="1">
         <v>0</v>
       </c>
     </row>
@@ -1781,7 +1784,7 @@
       <c r="A174">
         <v>20141220</v>
       </c>
-      <c r="B174">
+      <c r="B174" s="1">
         <v>0</v>
       </c>
     </row>
@@ -1789,7 +1792,7 @@
       <c r="A175">
         <v>20141221</v>
       </c>
-      <c r="B175">
+      <c r="B175" s="1">
         <v>0</v>
       </c>
     </row>
@@ -1797,7 +1800,7 @@
       <c r="A176">
         <v>20141222</v>
       </c>
-      <c r="B176">
+      <c r="B176" s="1">
         <v>0</v>
       </c>
     </row>
@@ -1805,7 +1808,7 @@
       <c r="A177">
         <v>20141223</v>
       </c>
-      <c r="B177">
+      <c r="B177" s="1">
         <v>0</v>
       </c>
     </row>
@@ -1813,7 +1816,7 @@
       <c r="A178">
         <v>20141224</v>
       </c>
-      <c r="B178">
+      <c r="B178" s="1">
         <v>0</v>
       </c>
     </row>
@@ -1821,7 +1824,7 @@
       <c r="A179">
         <v>20141225</v>
       </c>
-      <c r="B179">
+      <c r="B179" s="1">
         <v>0</v>
       </c>
     </row>
@@ -1829,7 +1832,7 @@
       <c r="A180">
         <v>20141226</v>
       </c>
-      <c r="B180">
+      <c r="B180" s="1">
         <v>0</v>
       </c>
     </row>
@@ -1837,7 +1840,7 @@
       <c r="A181">
         <v>20141227</v>
       </c>
-      <c r="B181">
+      <c r="B181" s="1">
         <v>0</v>
       </c>
     </row>
@@ -1845,7 +1848,7 @@
       <c r="A182">
         <v>20141228</v>
       </c>
-      <c r="B182">
+      <c r="B182" s="1">
         <v>0</v>
       </c>
     </row>
@@ -1853,7 +1856,7 @@
       <c r="A183">
         <v>20141229</v>
       </c>
-      <c r="B183">
+      <c r="B183" s="1">
         <v>0</v>
       </c>
     </row>
@@ -1861,7 +1864,7 @@
       <c r="A184">
         <v>20141230</v>
       </c>
-      <c r="B184">
+      <c r="B184" s="1">
         <v>0</v>
       </c>
     </row>
@@ -1869,15 +1872,15 @@
       <c r="A185">
         <v>20141231</v>
       </c>
-      <c r="B185">
-        <v>0</v>
+      <c r="B185" s="1">
+        <v>6.0000000000000001E-3</v>
       </c>
     </row>
     <row r="186" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A186">
         <v>20150101</v>
       </c>
-      <c r="B186">
+      <c r="B186" s="1">
         <v>0</v>
       </c>
     </row>
@@ -1885,7 +1888,7 @@
       <c r="A187">
         <v>20150102</v>
       </c>
-      <c r="B187">
+      <c r="B187" s="1">
         <v>0</v>
       </c>
     </row>
@@ -1893,7 +1896,7 @@
       <c r="A188">
         <v>20150103</v>
       </c>
-      <c r="B188">
+      <c r="B188" s="1">
         <v>0</v>
       </c>
     </row>
@@ -1901,7 +1904,7 @@
       <c r="A189">
         <v>20150104</v>
       </c>
-      <c r="B189">
+      <c r="B189" s="1">
         <v>0</v>
       </c>
     </row>
@@ -1909,7 +1912,7 @@
       <c r="A190">
         <v>20150105</v>
       </c>
-      <c r="B190">
+      <c r="B190" s="1">
         <v>0</v>
       </c>
     </row>
@@ -1917,7 +1920,7 @@
       <c r="A191">
         <v>20150106</v>
       </c>
-      <c r="B191">
+      <c r="B191" s="1">
         <v>0</v>
       </c>
     </row>
@@ -1925,7 +1928,7 @@
       <c r="A192">
         <v>20150107</v>
       </c>
-      <c r="B192">
+      <c r="B192" s="1">
         <v>0</v>
       </c>
     </row>
@@ -1933,7 +1936,7 @@
       <c r="A193">
         <v>20150108</v>
       </c>
-      <c r="B193">
+      <c r="B193" s="1">
         <v>0</v>
       </c>
     </row>
@@ -1941,7 +1944,7 @@
       <c r="A194">
         <v>20150109</v>
       </c>
-      <c r="B194">
+      <c r="B194" s="1">
         <v>0</v>
       </c>
     </row>
@@ -1949,7 +1952,7 @@
       <c r="A195">
         <v>20150110</v>
       </c>
-      <c r="B195">
+      <c r="B195" s="1">
         <v>0</v>
       </c>
     </row>
@@ -1957,7 +1960,7 @@
       <c r="A196">
         <v>20150111</v>
       </c>
-      <c r="B196">
+      <c r="B196" s="1">
         <v>0</v>
       </c>
     </row>
@@ -1965,7 +1968,7 @@
       <c r="A197">
         <v>20150112</v>
       </c>
-      <c r="B197">
+      <c r="B197" s="1">
         <v>0</v>
       </c>
     </row>
@@ -1973,7 +1976,7 @@
       <c r="A198">
         <v>20150113</v>
       </c>
-      <c r="B198">
+      <c r="B198" s="1">
         <v>0</v>
       </c>
     </row>
@@ -1981,7 +1984,7 @@
       <c r="A199">
         <v>20150114</v>
       </c>
-      <c r="B199">
+      <c r="B199" s="1">
         <v>0</v>
       </c>
     </row>
@@ -1989,7 +1992,7 @@
       <c r="A200">
         <v>20150115</v>
       </c>
-      <c r="B200">
+      <c r="B200" s="1">
         <v>0</v>
       </c>
     </row>
@@ -1997,7 +2000,7 @@
       <c r="A201">
         <v>20150116</v>
       </c>
-      <c r="B201">
+      <c r="B201" s="1">
         <v>0</v>
       </c>
     </row>
@@ -2005,7 +2008,7 @@
       <c r="A202">
         <v>20150117</v>
       </c>
-      <c r="B202">
+      <c r="B202" s="1">
         <v>0</v>
       </c>
     </row>
@@ -2013,7 +2016,7 @@
       <c r="A203">
         <v>20150118</v>
       </c>
-      <c r="B203">
+      <c r="B203" s="1">
         <v>0</v>
       </c>
     </row>
@@ -2021,7 +2024,7 @@
       <c r="A204">
         <v>20150119</v>
       </c>
-      <c r="B204">
+      <c r="B204" s="1">
         <v>0</v>
       </c>
     </row>
@@ -2029,7 +2032,7 @@
       <c r="A205">
         <v>20150120</v>
       </c>
-      <c r="B205">
+      <c r="B205" s="1">
         <v>0</v>
       </c>
     </row>
@@ -2037,7 +2040,7 @@
       <c r="A206">
         <v>20150121</v>
       </c>
-      <c r="B206">
+      <c r="B206" s="1">
         <v>0</v>
       </c>
     </row>
@@ -2045,7 +2048,7 @@
       <c r="A207">
         <v>20150122</v>
       </c>
-      <c r="B207">
+      <c r="B207" s="1">
         <v>0</v>
       </c>
     </row>
@@ -2053,7 +2056,7 @@
       <c r="A208">
         <v>20150123</v>
       </c>
-      <c r="B208">
+      <c r="B208" s="1">
         <v>0</v>
       </c>
     </row>
@@ -2061,7 +2064,7 @@
       <c r="A209">
         <v>20150124</v>
       </c>
-      <c r="B209">
+      <c r="B209" s="1">
         <v>0</v>
       </c>
     </row>
@@ -2069,7 +2072,7 @@
       <c r="A210">
         <v>20150125</v>
       </c>
-      <c r="B210">
+      <c r="B210" s="1">
         <v>0</v>
       </c>
     </row>
@@ -2077,7 +2080,7 @@
       <c r="A211">
         <v>20150126</v>
       </c>
-      <c r="B211">
+      <c r="B211" s="1">
         <v>0</v>
       </c>
     </row>
@@ -2085,7 +2088,7 @@
       <c r="A212">
         <v>20150127</v>
       </c>
-      <c r="B212">
+      <c r="B212" s="1">
         <v>0</v>
       </c>
     </row>
@@ -2093,7 +2096,7 @@
       <c r="A213">
         <v>20150128</v>
       </c>
-      <c r="B213">
+      <c r="B213" s="1">
         <v>0</v>
       </c>
     </row>
@@ -2101,7 +2104,7 @@
       <c r="A214">
         <v>20150129</v>
       </c>
-      <c r="B214">
+      <c r="B214" s="1">
         <v>0</v>
       </c>
     </row>
@@ -2109,7 +2112,7 @@
       <c r="A215">
         <v>20150130</v>
       </c>
-      <c r="B215">
+      <c r="B215" s="1">
         <v>0</v>
       </c>
     </row>
@@ -2117,7 +2120,7 @@
       <c r="A216">
         <v>20150131</v>
       </c>
-      <c r="B216">
+      <c r="B216" s="1">
         <v>0</v>
       </c>
     </row>
@@ -2125,7 +2128,7 @@
       <c r="A217">
         <v>20150201</v>
       </c>
-      <c r="B217">
+      <c r="B217" s="1">
         <v>0</v>
       </c>
     </row>
@@ -2133,7 +2136,7 @@
       <c r="A218">
         <v>20150202</v>
       </c>
-      <c r="B218">
+      <c r="B218" s="1">
         <v>0</v>
       </c>
     </row>
@@ -2141,7 +2144,7 @@
       <c r="A219">
         <v>20150203</v>
       </c>
-      <c r="B219">
+      <c r="B219" s="1">
         <v>0</v>
       </c>
     </row>
@@ -2149,7 +2152,7 @@
       <c r="A220">
         <v>20150204</v>
       </c>
-      <c r="B220">
+      <c r="B220" s="1">
         <v>0</v>
       </c>
     </row>
@@ -2157,7 +2160,7 @@
       <c r="A221">
         <v>20150205</v>
       </c>
-      <c r="B221">
+      <c r="B221" s="1">
         <v>0</v>
       </c>
     </row>
@@ -2165,7 +2168,7 @@
       <c r="A222">
         <v>20150206</v>
       </c>
-      <c r="B222">
+      <c r="B222" s="1">
         <v>0</v>
       </c>
     </row>
@@ -2173,7 +2176,7 @@
       <c r="A223">
         <v>20150207</v>
       </c>
-      <c r="B223">
+      <c r="B223" s="1">
         <v>0</v>
       </c>
     </row>
@@ -2181,7 +2184,7 @@
       <c r="A224">
         <v>20150208</v>
       </c>
-      <c r="B224">
+      <c r="B224" s="1">
         <v>0</v>
       </c>
     </row>
@@ -2189,7 +2192,7 @@
       <c r="A225">
         <v>20150209</v>
       </c>
-      <c r="B225">
+      <c r="B225" s="1">
         <v>0</v>
       </c>
     </row>
@@ -2197,15 +2200,15 @@
       <c r="A226">
         <v>20150210</v>
       </c>
-      <c r="B226">
-        <v>0</v>
+      <c r="B226" s="1">
+        <v>1E-3</v>
       </c>
     </row>
     <row r="227" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A227">
         <v>20150211</v>
       </c>
-      <c r="B227">
+      <c r="B227" s="1">
         <v>0</v>
       </c>
     </row>
@@ -2213,7 +2216,7 @@
       <c r="A228">
         <v>20150212</v>
       </c>
-      <c r="B228">
+      <c r="B228" s="1">
         <v>0</v>
       </c>
     </row>
@@ -2221,7 +2224,7 @@
       <c r="A229">
         <v>20150213</v>
       </c>
-      <c r="B229">
+      <c r="B229" s="1">
         <v>0</v>
       </c>
     </row>
@@ -2229,15 +2232,15 @@
       <c r="A230">
         <v>20150214</v>
       </c>
-      <c r="B230">
-        <v>0</v>
+      <c r="B230" s="1">
+        <v>1.7000000000000001E-2</v>
       </c>
     </row>
     <row r="231" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A231">
         <v>20150215</v>
       </c>
-      <c r="B231">
+      <c r="B231" s="1">
         <v>0</v>
       </c>
     </row>
@@ -2245,7 +2248,7 @@
       <c r="A232">
         <v>20150216</v>
       </c>
-      <c r="B232">
+      <c r="B232" s="1">
         <v>0</v>
       </c>
     </row>
@@ -2253,7 +2256,7 @@
       <c r="A233">
         <v>20150217</v>
       </c>
-      <c r="B233">
+      <c r="B233" s="1">
         <v>0</v>
       </c>
     </row>
@@ -2261,23 +2264,23 @@
       <c r="A234">
         <v>20150218</v>
       </c>
-      <c r="B234">
-        <v>0</v>
+      <c r="B234" s="1">
+        <v>0.01</v>
       </c>
     </row>
     <row r="235" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A235">
         <v>20150219</v>
       </c>
-      <c r="B235">
-        <v>0</v>
+      <c r="B235" s="1">
+        <v>0.28399999999999997</v>
       </c>
     </row>
     <row r="236" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A236">
         <v>20150220</v>
       </c>
-      <c r="B236">
+      <c r="B236" s="1">
         <v>0</v>
       </c>
     </row>
@@ -2285,7 +2288,7 @@
       <c r="A237">
         <v>20150221</v>
       </c>
-      <c r="B237">
+      <c r="B237" s="1">
         <v>0</v>
       </c>
     </row>
@@ -2293,7 +2296,7 @@
       <c r="A238">
         <v>20150222</v>
       </c>
-      <c r="B238">
+      <c r="B238" s="1">
         <v>0</v>
       </c>
     </row>
@@ -2301,7 +2304,7 @@
       <c r="A239">
         <v>20150223</v>
       </c>
-      <c r="B239">
+      <c r="B239" s="1">
         <v>0</v>
       </c>
     </row>
@@ -2309,15 +2312,15 @@
       <c r="A240">
         <v>20150224</v>
       </c>
-      <c r="B240">
-        <v>0</v>
+      <c r="B240" s="1">
+        <v>4.0000000000000001E-3</v>
       </c>
     </row>
     <row r="241" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A241">
         <v>20150225</v>
       </c>
-      <c r="B241">
+      <c r="B241" s="1">
         <v>0</v>
       </c>
     </row>
@@ -2325,7 +2328,7 @@
       <c r="A242">
         <v>20150226</v>
       </c>
-      <c r="B242">
+      <c r="B242" s="1">
         <v>0</v>
       </c>
     </row>
@@ -2333,7 +2336,7 @@
       <c r="A243">
         <v>20150227</v>
       </c>
-      <c r="B243">
+      <c r="B243" s="1">
         <v>0</v>
       </c>
     </row>
@@ -2341,7 +2344,7 @@
       <c r="A244">
         <v>20150228</v>
       </c>
-      <c r="B244">
+      <c r="B244" s="1">
         <v>0</v>
       </c>
     </row>
@@ -2349,7 +2352,7 @@
       <c r="A245">
         <v>20150301</v>
       </c>
-      <c r="B245">
+      <c r="B245" s="1">
         <v>0</v>
       </c>
     </row>
@@ -2357,7 +2360,7 @@
       <c r="A246">
         <v>20150302</v>
       </c>
-      <c r="B246">
+      <c r="B246" s="1">
         <v>0</v>
       </c>
     </row>
@@ -2365,7 +2368,7 @@
       <c r="A247">
         <v>20150303</v>
       </c>
-      <c r="B247">
+      <c r="B247" s="1">
         <v>0</v>
       </c>
     </row>
@@ -2373,7 +2376,7 @@
       <c r="A248">
         <v>20150304</v>
       </c>
-      <c r="B248">
+      <c r="B248" s="1">
         <v>0</v>
       </c>
     </row>
@@ -2381,7 +2384,7 @@
       <c r="A249">
         <v>20150305</v>
       </c>
-      <c r="B249">
+      <c r="B249" s="1">
         <v>0</v>
       </c>
     </row>
@@ -2389,7 +2392,7 @@
       <c r="A250">
         <v>20150306</v>
       </c>
-      <c r="B250">
+      <c r="B250" s="1">
         <v>0</v>
       </c>
     </row>
@@ -2397,7 +2400,7 @@
       <c r="A251">
         <v>20150307</v>
       </c>
-      <c r="B251">
+      <c r="B251" s="1">
         <v>0</v>
       </c>
     </row>
@@ -2405,7 +2408,7 @@
       <c r="A252">
         <v>20150308</v>
       </c>
-      <c r="B252">
+      <c r="B252" s="1">
         <v>0</v>
       </c>
     </row>
@@ -2413,7 +2416,7 @@
       <c r="A253">
         <v>20150309</v>
       </c>
-      <c r="B253">
+      <c r="B253" s="1">
         <v>0</v>
       </c>
     </row>
@@ -2421,7 +2424,7 @@
       <c r="A254">
         <v>20150310</v>
       </c>
-      <c r="B254">
+      <c r="B254" s="1">
         <v>0</v>
       </c>
     </row>
@@ -2429,7 +2432,7 @@
       <c r="A255">
         <v>20150311</v>
       </c>
-      <c r="B255">
+      <c r="B255" s="1">
         <v>0</v>
       </c>
     </row>
@@ -2437,7 +2440,7 @@
       <c r="A256">
         <v>20150312</v>
       </c>
-      <c r="B256">
+      <c r="B256" s="1">
         <v>0</v>
       </c>
     </row>
@@ -2445,7 +2448,7 @@
       <c r="A257">
         <v>20150313</v>
       </c>
-      <c r="B257">
+      <c r="B257" s="1">
         <v>0</v>
       </c>
     </row>
@@ -2453,7 +2456,7 @@
       <c r="A258">
         <v>20150314</v>
       </c>
-      <c r="B258">
+      <c r="B258" s="1">
         <v>0</v>
       </c>
     </row>
@@ -2461,7 +2464,7 @@
       <c r="A259">
         <v>20150315</v>
       </c>
-      <c r="B259">
+      <c r="B259" s="1">
         <v>0</v>
       </c>
     </row>
@@ -2469,7 +2472,7 @@
       <c r="A260">
         <v>20150316</v>
       </c>
-      <c r="B260">
+      <c r="B260" s="1">
         <v>0</v>
       </c>
     </row>
@@ -2477,15 +2480,15 @@
       <c r="A261">
         <v>20150317</v>
       </c>
-      <c r="B261">
-        <v>0</v>
+      <c r="B261" s="1">
+        <v>1E-3</v>
       </c>
     </row>
     <row r="262" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A262">
         <v>20150318</v>
       </c>
-      <c r="B262">
+      <c r="B262" s="1">
         <v>0</v>
       </c>
     </row>
@@ -2493,31 +2496,31 @@
       <c r="A263">
         <v>20150319</v>
       </c>
-      <c r="B263">
-        <v>0</v>
+      <c r="B263" s="1">
+        <v>8.0000000000000002E-3</v>
       </c>
     </row>
     <row r="264" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A264">
         <v>20150320</v>
       </c>
-      <c r="B264">
-        <v>0</v>
+      <c r="B264" s="1">
+        <v>1.7000000000000001E-2</v>
       </c>
     </row>
     <row r="265" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A265">
         <v>20150321</v>
       </c>
-      <c r="B265">
-        <v>0</v>
+      <c r="B265" s="1">
+        <v>4.7E-2</v>
       </c>
     </row>
     <row r="266" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A266">
         <v>20150322</v>
       </c>
-      <c r="B266">
+      <c r="B266" s="1">
         <v>0</v>
       </c>
     </row>
@@ -2525,7 +2528,7 @@
       <c r="A267">
         <v>20150323</v>
       </c>
-      <c r="B267">
+      <c r="B267" s="1">
         <v>0</v>
       </c>
     </row>
@@ -2533,7 +2536,7 @@
       <c r="A268">
         <v>20150324</v>
       </c>
-      <c r="B268">
+      <c r="B268" s="1">
         <v>0</v>
       </c>
     </row>
@@ -2541,7 +2544,7 @@
       <c r="A269">
         <v>20150325</v>
       </c>
-      <c r="B269">
+      <c r="B269" s="1">
         <v>0</v>
       </c>
     </row>
@@ -2549,7 +2552,7 @@
       <c r="A270">
         <v>20150326</v>
       </c>
-      <c r="B270">
+      <c r="B270" s="1">
         <v>0</v>
       </c>
     </row>
@@ -2557,7 +2560,7 @@
       <c r="A271">
         <v>20150327</v>
       </c>
-      <c r="B271">
+      <c r="B271" s="1">
         <v>0</v>
       </c>
     </row>
@@ -2565,7 +2568,7 @@
       <c r="A272">
         <v>20150328</v>
       </c>
-      <c r="B272">
+      <c r="B272" s="1">
         <v>0</v>
       </c>
     </row>
@@ -2573,7 +2576,7 @@
       <c r="A273">
         <v>20150329</v>
       </c>
-      <c r="B273">
+      <c r="B273" s="1">
         <v>0</v>
       </c>
     </row>
@@ -2581,7 +2584,7 @@
       <c r="A274">
         <v>20150330</v>
       </c>
-      <c r="B274">
+      <c r="B274" s="1">
         <v>0</v>
       </c>
     </row>
@@ -2589,7 +2592,7 @@
       <c r="A275">
         <v>20150331</v>
       </c>
-      <c r="B275">
+      <c r="B275" s="1">
         <v>0</v>
       </c>
     </row>
@@ -2597,7 +2600,7 @@
       <c r="A276">
         <v>20150401</v>
       </c>
-      <c r="B276">
+      <c r="B276" s="1">
         <v>0</v>
       </c>
     </row>
@@ -2605,7 +2608,7 @@
       <c r="A277">
         <v>20150402</v>
       </c>
-      <c r="B277">
+      <c r="B277" s="1">
         <v>0</v>
       </c>
     </row>
@@ -2613,7 +2616,7 @@
       <c r="A278">
         <v>20150403</v>
       </c>
-      <c r="B278">
+      <c r="B278" s="1">
         <v>0</v>
       </c>
     </row>
@@ -2621,15 +2624,15 @@
       <c r="A279">
         <v>20150404</v>
       </c>
-      <c r="B279">
-        <v>0</v>
+      <c r="B279" s="1">
+        <v>6.5000000000000002E-2</v>
       </c>
     </row>
     <row r="280" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A280">
         <v>20150405</v>
       </c>
-      <c r="B280">
+      <c r="B280" s="1">
         <v>0</v>
       </c>
     </row>
@@ -2637,7 +2640,7 @@
       <c r="A281">
         <v>20150406</v>
       </c>
-      <c r="B281">
+      <c r="B281" s="1">
         <v>0</v>
       </c>
     </row>
@@ -2645,7 +2648,7 @@
       <c r="A282">
         <v>20150407</v>
       </c>
-      <c r="B282">
+      <c r="B282" s="1">
         <v>0</v>
       </c>
     </row>
@@ -2653,7 +2656,7 @@
       <c r="A283">
         <v>20150408</v>
       </c>
-      <c r="B283">
+      <c r="B283" s="1">
         <v>0</v>
       </c>
     </row>
@@ -2661,7 +2664,7 @@
       <c r="A284">
         <v>20150409</v>
       </c>
-      <c r="B284">
+      <c r="B284" s="1">
         <v>0</v>
       </c>
     </row>
@@ -2669,7 +2672,7 @@
       <c r="A285">
         <v>20150410</v>
       </c>
-      <c r="B285">
+      <c r="B285" s="1">
         <v>0</v>
       </c>
     </row>
@@ -2677,7 +2680,7 @@
       <c r="A286">
         <v>20150411</v>
       </c>
-      <c r="B286">
+      <c r="B286" s="1">
         <v>0</v>
       </c>
     </row>
@@ -2685,7 +2688,7 @@
       <c r="A287">
         <v>20150412</v>
       </c>
-      <c r="B287">
+      <c r="B287" s="1">
         <v>0</v>
       </c>
     </row>
@@ -2693,7 +2696,7 @@
       <c r="A288">
         <v>20150413</v>
       </c>
-      <c r="B288">
+      <c r="B288" s="1">
         <v>0</v>
       </c>
     </row>
@@ -2701,7 +2704,7 @@
       <c r="A289">
         <v>20150414</v>
       </c>
-      <c r="B289">
+      <c r="B289" s="1">
         <v>0</v>
       </c>
     </row>
@@ -2709,7 +2712,7 @@
       <c r="A290">
         <v>20150415</v>
       </c>
-      <c r="B290">
+      <c r="B290" s="1">
         <v>0</v>
       </c>
     </row>
@@ -2717,7 +2720,7 @@
       <c r="A291">
         <v>20150416</v>
       </c>
-      <c r="B291">
+      <c r="B291" s="1">
         <v>0</v>
       </c>
     </row>
@@ -2725,7 +2728,7 @@
       <c r="A292">
         <v>20150417</v>
       </c>
-      <c r="B292">
+      <c r="B292" s="1">
         <v>0</v>
       </c>
     </row>
@@ -2733,7 +2736,7 @@
       <c r="A293">
         <v>20150418</v>
       </c>
-      <c r="B293">
+      <c r="B293" s="1">
         <v>0</v>
       </c>
     </row>
@@ -2741,7 +2744,7 @@
       <c r="A294">
         <v>20150419</v>
       </c>
-      <c r="B294">
+      <c r="B294" s="1">
         <v>0</v>
       </c>
     </row>
@@ -2749,7 +2752,7 @@
       <c r="A295">
         <v>20150420</v>
       </c>
-      <c r="B295">
+      <c r="B295" s="1">
         <v>0</v>
       </c>
     </row>
@@ -2757,7 +2760,7 @@
       <c r="A296">
         <v>20150421</v>
       </c>
-      <c r="B296">
+      <c r="B296" s="1">
         <v>0</v>
       </c>
     </row>
@@ -2765,7 +2768,7 @@
       <c r="A297">
         <v>20150422</v>
       </c>
-      <c r="B297">
+      <c r="B297" s="1">
         <v>0</v>
       </c>
     </row>
@@ -2773,7 +2776,7 @@
       <c r="A298">
         <v>20150423</v>
       </c>
-      <c r="B298">
+      <c r="B298" s="1">
         <v>0</v>
       </c>
     </row>
@@ -2781,39 +2784,39 @@
       <c r="A299">
         <v>20150424</v>
       </c>
-      <c r="B299">
-        <v>0</v>
+      <c r="B299" s="1">
+        <v>0.191</v>
       </c>
     </row>
     <row r="300" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A300">
         <v>20150425</v>
       </c>
-      <c r="B300">
-        <v>0</v>
+      <c r="B300" s="1">
+        <v>0.32500000000000001</v>
       </c>
     </row>
     <row r="301" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A301">
         <v>20150426</v>
       </c>
-      <c r="B301">
-        <v>0</v>
+      <c r="B301" s="1">
+        <v>6.6360000000000001</v>
       </c>
     </row>
     <row r="302" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A302">
         <v>20150427</v>
       </c>
-      <c r="B302">
-        <v>0</v>
+      <c r="B302" s="1">
+        <v>1.3540000000000001</v>
       </c>
     </row>
     <row r="303" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A303">
         <v>20150428</v>
       </c>
-      <c r="B303">
+      <c r="B303" s="1">
         <v>0</v>
       </c>
     </row>
@@ -2821,7 +2824,7 @@
       <c r="A304">
         <v>20150429</v>
       </c>
-      <c r="B304">
+      <c r="B304" s="1">
         <v>0</v>
       </c>
     </row>
@@ -2829,7 +2832,7 @@
       <c r="A305">
         <v>20150430</v>
       </c>
-      <c r="B305">
+      <c r="B305" s="1">
         <v>0</v>
       </c>
     </row>
@@ -2837,7 +2840,7 @@
       <c r="A306">
         <v>20150501</v>
       </c>
-      <c r="B306">
+      <c r="B306" s="1">
         <v>0</v>
       </c>
     </row>
@@ -2845,7 +2848,7 @@
       <c r="A307">
         <v>20150502</v>
       </c>
-      <c r="B307">
+      <c r="B307" s="1">
         <v>0</v>
       </c>
     </row>
@@ -2853,71 +2856,71 @@
       <c r="A308">
         <v>20150503</v>
       </c>
-      <c r="B308">
-        <v>0</v>
+      <c r="B308" s="1">
+        <v>4.0350000000000001</v>
       </c>
     </row>
     <row r="309" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A309">
         <v>20150504</v>
       </c>
-      <c r="B309">
-        <v>0</v>
+      <c r="B309" s="1">
+        <v>5.3540000000000001</v>
       </c>
     </row>
     <row r="310" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A310">
         <v>20150505</v>
       </c>
-      <c r="B310">
-        <v>0</v>
+      <c r="B310" s="1">
+        <v>22.962</v>
       </c>
     </row>
     <row r="311" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A311">
         <v>20150506</v>
       </c>
-      <c r="B311">
-        <v>0</v>
+      <c r="B311" s="1">
+        <v>8.1739999999999995</v>
       </c>
     </row>
     <row r="312" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A312">
         <v>20150507</v>
       </c>
-      <c r="B312">
-        <v>0</v>
+      <c r="B312" s="1">
+        <v>15.566000000000001</v>
       </c>
     </row>
     <row r="313" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A313">
         <v>20150508</v>
       </c>
-      <c r="B313">
-        <v>0</v>
+      <c r="B313" s="1">
+        <v>8.4979999999999993</v>
       </c>
     </row>
     <row r="314" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A314">
         <v>20150509</v>
       </c>
-      <c r="B314">
-        <v>0</v>
+      <c r="B314" s="1">
+        <v>6.694</v>
       </c>
     </row>
     <row r="315" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A315">
         <v>20150510</v>
       </c>
-      <c r="B315">
-        <v>0</v>
+      <c r="B315" s="1">
+        <v>1E-3</v>
       </c>
     </row>
     <row r="316" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A316">
         <v>20150511</v>
       </c>
-      <c r="B316">
+      <c r="B316" s="1">
         <v>0</v>
       </c>
     </row>
@@ -2925,15 +2928,15 @@
       <c r="A317">
         <v>20150512</v>
       </c>
-      <c r="B317">
-        <v>0</v>
+      <c r="B317" s="1">
+        <v>3.5000000000000003E-2</v>
       </c>
     </row>
     <row r="318" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A318">
         <v>20150513</v>
       </c>
-      <c r="B318">
+      <c r="B318" s="1">
         <v>0</v>
       </c>
     </row>
@@ -2941,7 +2944,7 @@
       <c r="A319">
         <v>20150514</v>
       </c>
-      <c r="B319">
+      <c r="B319" s="1">
         <v>0</v>
       </c>
     </row>
@@ -2949,7 +2952,7 @@
       <c r="A320">
         <v>20150515</v>
       </c>
-      <c r="B320">
+      <c r="B320" s="1">
         <v>0</v>
       </c>
     </row>
@@ -2957,7 +2960,7 @@
       <c r="A321">
         <v>20150516</v>
       </c>
-      <c r="B321">
+      <c r="B321" s="1">
         <v>0</v>
       </c>
     </row>
@@ -2965,15 +2968,15 @@
       <c r="A322">
         <v>20150517</v>
       </c>
-      <c r="B322">
-        <v>0</v>
+      <c r="B322" s="1">
+        <v>5.0000000000000001E-3</v>
       </c>
     </row>
     <row r="323" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A323">
         <v>20150518</v>
       </c>
-      <c r="B323">
+      <c r="B323" s="1">
         <v>0</v>
       </c>
     </row>
@@ -2981,15 +2984,15 @@
       <c r="A324">
         <v>20150519</v>
       </c>
-      <c r="B324">
-        <v>0</v>
+      <c r="B324" s="1">
+        <v>1.6E-2</v>
       </c>
     </row>
     <row r="325" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A325">
         <v>20150520</v>
       </c>
-      <c r="B325">
+      <c r="B325" s="1">
         <v>0</v>
       </c>
     </row>
@@ -2997,15 +3000,15 @@
       <c r="A326">
         <v>20150521</v>
       </c>
-      <c r="B326">
-        <v>0</v>
+      <c r="B326" s="1">
+        <v>1.847</v>
       </c>
     </row>
     <row r="327" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A327">
         <v>20150522</v>
       </c>
-      <c r="B327">
+      <c r="B327" s="1">
         <v>0</v>
       </c>
     </row>
@@ -3013,87 +3016,87 @@
       <c r="A328">
         <v>20150523</v>
       </c>
-      <c r="B328">
-        <v>0</v>
+      <c r="B328" s="1">
+        <v>2.1000000000000001E-2</v>
       </c>
     </row>
     <row r="329" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A329">
         <v>20150524</v>
       </c>
-      <c r="B329">
-        <v>0</v>
+      <c r="B329" s="1">
+        <v>8.9999999999999993E-3</v>
       </c>
     </row>
     <row r="330" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A330">
         <v>20150525</v>
       </c>
-      <c r="B330">
-        <v>0</v>
+      <c r="B330" s="1">
+        <v>0.497</v>
       </c>
     </row>
     <row r="331" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A331">
         <v>20150526</v>
       </c>
-      <c r="B331">
-        <v>0</v>
+      <c r="B331" s="1">
+        <v>8.8000000000000007</v>
       </c>
     </row>
     <row r="332" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A332">
         <v>20150527</v>
       </c>
-      <c r="B332">
-        <v>0</v>
+      <c r="B332" s="1">
+        <v>12.929</v>
       </c>
     </row>
     <row r="333" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A333">
         <v>20150528</v>
       </c>
-      <c r="B333">
-        <v>0</v>
+      <c r="B333" s="1">
+        <v>7.7240000000000002</v>
       </c>
     </row>
     <row r="334" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A334">
         <v>20150529</v>
       </c>
-      <c r="B334">
-        <v>0</v>
+      <c r="B334" s="1">
+        <v>1.8080000000000001</v>
       </c>
     </row>
     <row r="335" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A335">
         <v>20150530</v>
       </c>
-      <c r="B335">
-        <v>0</v>
+      <c r="B335" s="1">
+        <v>0.23200000000000001</v>
       </c>
     </row>
     <row r="336" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A336">
         <v>20150531</v>
       </c>
-      <c r="B336">
-        <v>0</v>
+      <c r="B336" s="1">
+        <v>4.4999999999999998E-2</v>
       </c>
     </row>
     <row r="337" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A337">
         <v>20150601</v>
       </c>
-      <c r="B337">
-        <v>0</v>
+      <c r="B337" s="1">
+        <v>0.13700000000000001</v>
       </c>
     </row>
     <row r="338" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A338">
         <v>20150602</v>
       </c>
-      <c r="B338">
+      <c r="B338" s="1">
         <v>0</v>
       </c>
     </row>
@@ -3101,7 +3104,7 @@
       <c r="A339">
         <v>20150603</v>
       </c>
-      <c r="B339">
+      <c r="B339" s="1">
         <v>0</v>
       </c>
     </row>
@@ -3109,15 +3112,15 @@
       <c r="A340">
         <v>20150604</v>
       </c>
-      <c r="B340">
-        <v>0</v>
+      <c r="B340" s="1">
+        <v>1.9E-2</v>
       </c>
     </row>
     <row r="341" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A341">
         <v>20150605</v>
       </c>
-      <c r="B341">
+      <c r="B341" s="1">
         <v>0</v>
       </c>
     </row>
@@ -3125,7 +3128,7 @@
       <c r="A342">
         <v>20150606</v>
       </c>
-      <c r="B342">
+      <c r="B342" s="1">
         <v>0</v>
       </c>
     </row>
@@ -3133,192 +3136,192 @@
       <c r="A343">
         <v>20150607</v>
       </c>
-      <c r="B343">
-        <v>0</v>
+      <c r="B343" s="1">
+        <v>0.40600000000000003</v>
       </c>
     </row>
     <row r="344" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A344">
         <v>20150608</v>
       </c>
-      <c r="B344">
-        <v>0</v>
+      <c r="B344" s="1">
+        <v>0.98499999999999999</v>
       </c>
     </row>
     <row r="345" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A345">
         <v>20150609</v>
       </c>
-      <c r="B345">
-        <v>0</v>
+      <c r="B345" s="1">
+        <v>1.05</v>
       </c>
     </row>
     <row r="346" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A346">
         <v>20150610</v>
       </c>
-      <c r="B346">
-        <v>0</v>
+      <c r="B346" s="1">
+        <v>1.712</v>
       </c>
     </row>
     <row r="347" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A347">
         <v>20150611</v>
       </c>
-      <c r="B347">
-        <v>0</v>
+      <c r="B347" s="1">
+        <v>3.93</v>
       </c>
     </row>
     <row r="348" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A348">
         <v>20150612</v>
       </c>
-      <c r="B348">
-        <v>0</v>
+      <c r="B348" s="1">
+        <v>4.319</v>
       </c>
     </row>
     <row r="349" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A349">
         <v>20150613</v>
       </c>
-      <c r="B349">
-        <v>0</v>
+      <c r="B349" s="1">
+        <v>1.6E-2</v>
       </c>
     </row>
     <row r="350" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A350">
         <v>20150614</v>
       </c>
-      <c r="B350">
-        <v>0</v>
+      <c r="B350" s="1">
+        <v>8.5419999999999998</v>
       </c>
     </row>
     <row r="351" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A351">
         <v>20150615</v>
       </c>
-      <c r="B351">
-        <v>0</v>
+      <c r="B351" s="1">
+        <v>6.5880000000000001</v>
       </c>
     </row>
     <row r="352" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A352">
         <v>20150616</v>
       </c>
-      <c r="B352">
-        <v>0</v>
+      <c r="B352" s="1">
+        <v>0.128</v>
       </c>
     </row>
     <row r="353" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A353">
         <v>20150617</v>
       </c>
-      <c r="B353">
-        <v>0</v>
+      <c r="B353" s="1">
+        <v>1.0569999999999999</v>
       </c>
     </row>
     <row r="354" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A354">
         <v>20150618</v>
       </c>
-      <c r="B354">
-        <v>0</v>
+      <c r="B354" s="1">
+        <v>10.374000000000001</v>
       </c>
     </row>
     <row r="355" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A355">
         <v>20150619</v>
       </c>
-      <c r="B355">
-        <v>0</v>
+      <c r="B355" s="1">
+        <v>5.5369999999999999</v>
       </c>
     </row>
     <row r="356" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A356">
         <v>20150620</v>
       </c>
-      <c r="B356">
-        <v>0</v>
+      <c r="B356" s="1">
+        <v>8.4130000000000003</v>
       </c>
     </row>
     <row r="357" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A357">
         <v>20150621</v>
       </c>
-      <c r="B357">
-        <v>0</v>
+      <c r="B357" s="1">
+        <v>17.420999999999999</v>
       </c>
     </row>
     <row r="358" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A358">
         <v>20150622</v>
       </c>
-      <c r="B358">
-        <v>0</v>
+      <c r="B358" s="1">
+        <v>14.303000000000001</v>
       </c>
     </row>
     <row r="359" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A359">
         <v>20150623</v>
       </c>
-      <c r="B359">
-        <v>0</v>
+      <c r="B359" s="1">
+        <v>3.3439999999999999</v>
       </c>
     </row>
     <row r="360" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A360">
         <v>20150624</v>
       </c>
-      <c r="B360">
-        <v>0</v>
+      <c r="B360" s="1">
+        <v>5.9790000000000001</v>
       </c>
     </row>
     <row r="361" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A361">
         <v>20150625</v>
       </c>
-      <c r="B361">
-        <v>0</v>
+      <c r="B361" s="1">
+        <v>4.0119999999999996</v>
       </c>
     </row>
     <row r="362" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A362">
         <v>20150626</v>
       </c>
-      <c r="B362">
-        <v>0</v>
+      <c r="B362" s="1">
+        <v>1.105</v>
       </c>
     </row>
     <row r="363" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A363">
         <v>20150627</v>
       </c>
-      <c r="B363">
-        <v>0</v>
+      <c r="B363" s="1">
+        <v>2.464</v>
       </c>
     </row>
     <row r="364" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A364">
         <v>20150628</v>
       </c>
-      <c r="B364">
-        <v>0</v>
+      <c r="B364" s="1">
+        <v>2.1309999999999998</v>
       </c>
     </row>
     <row r="365" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A365">
         <v>20150629</v>
       </c>
-      <c r="B365">
-        <v>0</v>
+      <c r="B365" s="1">
+        <v>2.8010000000000002</v>
       </c>
     </row>
     <row r="366" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A366">
         <v>20150630</v>
       </c>
-      <c r="B366">
-        <v>0</v>
+      <c r="B366" s="1">
+        <v>1.903</v>
       </c>
     </row>
   </sheetData>

</xml_diff>